<commit_message>
Update trading fee rate
</commit_message>
<xml_diff>
--- a/docs/feeStructure/USDTFuturesTradingFeeRate.xlsx
+++ b/docs/feeStructure/USDTFuturesTradingFeeRate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samyakjain/Documents/Projects/Github/CryptoFuturesCalculator/docs/feeStructure/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{19AB958A-E4B6-444B-A6A6-854F822DA85D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6349E291-B3AD-294C-A057-1F15FBE0E7CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{9F69D791-F92B-0046-92D4-4B8BD46AEBC1}"/>
+    <workbookView xWindow="33600" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{9F69D791-F92B-0046-92D4-4B8BD46AEBC1}"/>
   </bookViews>
   <sheets>
     <sheet name="USDTFuturesTradingFeeRate" sheetId="1" r:id="rId1"/>
@@ -39,10 +39,10 @@
     <t>Level</t>
   </si>
   <si>
-    <t>Maker</t>
+    <t>Maker(%)</t>
   </si>
   <si>
-    <t>Taker</t>
+    <t>Taker(%)</t>
   </si>
 </sst>
 </file>
@@ -411,7 +411,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>